<commit_message>
Update files related calibration tool, some ideas regarding the user panel, plot data and send calibration
</commit_message>
<xml_diff>
--- a/CDI_code/Hardware/Hardware_Description_v2.xlsx
+++ b/CDI_code/Hardware/Hardware_Description_v2.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A551633\Documents\My_Dev_Repo\Repo\CDI\CDI_code\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev_Fabio\CDIrepo\CDI_code\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1F6780-3963-44EC-B550-F57F44E66AE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F18DBC-C191-45DB-B5D8-8D84C1A9D9AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Pin_Description" sheetId="1" r:id="rId1"/>
-    <sheet name="HV_Interrupt" sheetId="12" r:id="rId2"/>
-    <sheet name="Capacitor_Energy" sheetId="11" r:id="rId3"/>
-    <sheet name="Sheet5" sheetId="13" r:id="rId4"/>
-    <sheet name="Sheet6" sheetId="14" r:id="rId5"/>
-    <sheet name="Sheet7" sheetId="15" r:id="rId6"/>
-    <sheet name="Backlog" sheetId="2" r:id="rId7"/>
+    <sheet name="Backlog" sheetId="2" r:id="rId1"/>
+    <sheet name="Pin_Description" sheetId="1" r:id="rId2"/>
+    <sheet name="HV_Interrupt" sheetId="12" r:id="rId3"/>
+    <sheet name="Capacitor_Energy" sheetId="11" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="13" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="14" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="15" r:id="rId7"/>
     <sheet name="Calculation" sheetId="3" r:id="rId8"/>
     <sheet name="Rengineering" sheetId="4" r:id="rId9"/>
     <sheet name="Sheet1" sheetId="8" r:id="rId10"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="269">
   <si>
     <t xml:space="preserve">Story </t>
   </si>
@@ -658,12 +658,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Prepare to be available Serial connection in prototype board</t>
-  </si>
-  <si>
-    <t>I need to create the hardware connection to use the serial port (USART2), because I will leave USART1 free to use to upload new software in Bluepill</t>
-  </si>
-  <si>
     <t>BLUEPILL_LED</t>
   </si>
   <si>
@@ -863,6 +857,36 @@
   </si>
   <si>
     <t>USART3_RX/I2C2_SDA</t>
+  </si>
+  <si>
+    <t>Calibration tool</t>
+  </si>
+  <si>
+    <t>I need to develop a elementar Calibration tool built in Python with basic functionalities like: Graphical panel with Engine Speed breakpoint (12 values), advance angle (12 values), basic sensor configuration (angle rate and border definition) , read diagnostic, reset diagnostic, read internal values, maybe create a graphical window to analyse data came from ECU</t>
+  </si>
+  <si>
+    <t>Temperature sensor</t>
+  </si>
+  <si>
+    <t>Create a code responsible to treat the temperature sensor (NTC resistor), create an array with 8 position to describe the temperature in function the voltage on resistor</t>
+  </si>
+  <si>
+    <t>Update all documentation to create a efficient historic about the project, hardware details (include a possibility to include a E2PROM I2C memory on the board), redraw the GND regarding VRS sensor and stuff</t>
+  </si>
+  <si>
+    <t>Update documentation</t>
+  </si>
+  <si>
+    <t>Provide useful information</t>
+  </si>
+  <si>
+    <t>Create the data structure to record information about the system in running time like: max engine speed, min and max voltage system, internal diagnostic, reset numbers (hardware reset, WDT and etc), create some useful counter to measure the system quality/accuracy or something like this...</t>
+  </si>
+  <si>
+    <t>Final product (Box and assembly)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish the aluminum box (cut and conncet the internal wires) </t>
   </si>
 </sst>
 </file>
@@ -8781,794 +8805,123 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.625" customWidth="1"/>
+    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.25" customWidth="1"/>
+    <col min="3" max="3" width="46.75" customWidth="1"/>
+    <col min="4" max="4" width="16.375" customWidth="1"/>
+    <col min="5" max="5" width="30.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="30">
+        <v>44502</v>
+      </c>
+      <c r="B2" s="32" t="s">
         <v>259</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="C2" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F31" s="33" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F32" s="33" t="s">
-        <v>196</v>
-      </c>
-      <c r="H32" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
-        <v>41</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
-        <v>42</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
-        <v>43</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
-        <v>44</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
-        <v>45</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
-        <v>46</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
-        <v>47</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
-        <v>48</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E49" s="1"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="30">
+        <v>44502</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="30">
+        <v>44502</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+    </row>
+    <row r="5" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="30">
+        <v>44502</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+    </row>
+    <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="30">
+        <v>44502</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -21515,6 +20868,798 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="33" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="H32" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E49" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D4A6F7-0053-4B3B-ADA7-20EA37105384}">
   <dimension ref="A1:R29"/>
   <sheetViews>
@@ -21526,13 +21671,13 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="49" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B1" s="49"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B2" s="2">
         <v>9.9999999999999995E-7</v>
@@ -21540,7 +21685,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B3" s="2">
         <v>333</v>
@@ -21548,29 +21693,29 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B4" s="2">
         <v>1500000</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B5" s="2">
         <v>15000</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B6" s="36">
         <f>IF(B3*(B5/(B4+B5))&gt;3.3,3.3,B3*(B5/(B4+B5)))</f>
@@ -21579,32 +21724,32 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B8" s="2">
         <v>100000</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B9" s="2">
         <v>68000</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B10" s="2">
         <f>B9/(B8+B9)</f>
@@ -21617,98 +21762,98 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B12" s="2">
         <v>68000</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B13" s="2">
         <v>20000</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B15" s="2">
         <v>100000</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="L15" s="37"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B16" s="2">
         <v>1500000</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N16" s="37"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="F20" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="G20" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="I20" s="1" t="s">
+      <c r="K20" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="M20" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="K20" s="38" t="s">
+      <c r="N20" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="O20" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="P20" s="39" t="s">
         <v>239</v>
       </c>
-      <c r="O20" s="3" t="s">
+      <c r="Q20" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="P20" s="39" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>242</v>
-      </c>
       <c r="R20" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -21957,13 +22102,13 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
@@ -22023,11 +22168,12 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD39C8A0-CA37-4B5A-9204-4711E454FBBE}">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -22043,16 +22189,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B1" s="2">
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I1">
         <v>400</v>
@@ -22060,66 +22206,66 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B2" s="2">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="D2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E2">
         <v>94</v>
       </c>
       <c r="H2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I2" s="34">
         <v>5100000</v>
       </c>
       <c r="J2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B3" s="2">
         <v>300</v>
       </c>
       <c r="D3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E3">
         <v>93.98</v>
       </c>
       <c r="H3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I3" s="34">
         <v>43000</v>
       </c>
       <c r="J3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B4" s="2">
         <f>(B2*(B3^2))/2</f>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E4">
         <v>92.5</v>
       </c>
       <c r="H4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I4">
         <f>I1*(I3/(I2+I3))</f>
@@ -22128,14 +22274,14 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B5" s="2">
         <f>B3/B1</f>
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -22143,7 +22289,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E6">
         <f>91.5</f>
@@ -22165,10 +22311,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100F5C4D-205D-4BA5-B37A-C3D515743A6A}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -22183,7 +22330,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B1" s="2">
         <v>330000</v>
@@ -22191,7 +22338,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B2" s="2">
         <v>2200000</v>
@@ -22199,7 +22346,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B3" s="2">
         <v>1.41</v>
@@ -22207,7 +22354,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B4" s="2">
         <f>B3-0.1835</f>
@@ -22216,7 +22363,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -22224,7 +22371,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B6" s="2">
         <v>3.3</v>
@@ -22232,7 +22379,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B7" s="2">
         <f>((B1+B2)*B4-(B1*B5))/B2</f>
@@ -22241,7 +22388,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B8" s="2">
         <f>((B1+B2)*B4-(B1*B6))/B2</f>
@@ -22250,7 +22397,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B9" s="2">
         <f>B7-B8</f>
@@ -22259,7 +22406,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B10" s="2">
         <f>B1*(B6-B5)/B2</f>
@@ -22268,11 +22415,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2CD29A-2B20-4F70-8A3F-3E3ADB9F6627}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -22284,7 +22432,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B1">
         <v>3.3</v>
@@ -22292,7 +22440,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B2">
         <v>75000</v>
@@ -22300,7 +22448,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B3">
         <v>100000</v>
@@ -22308,7 +22456,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B4">
         <v>1.226</v>
@@ -22316,7 +22464,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B5">
         <v>330000</v>
@@ -22324,7 +22472,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B6">
         <v>2200000</v>
@@ -22332,7 +22480,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -22340,7 +22488,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B8">
         <v>3.3</v>
@@ -22348,7 +22496,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B9">
         <f>((B5+B6)*B4-(B5*B7))/B6</f>
@@ -22357,7 +22505,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B10">
         <f>((B5+B6)*B4-(B5*B8))/B6</f>
@@ -22366,7 +22514,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B11">
         <f>B9-B10</f>
@@ -22375,7 +22523,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B12">
         <f>B5*(B8-B7)/B6</f>
@@ -22384,11 +22532,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B809229D-9D44-4C7F-8241-DAEA6E4E24A3}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -22400,7 +22549,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B1">
         <v>1.226</v>
@@ -22408,7 +22557,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B2">
         <v>330000</v>
@@ -22416,7 +22565,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B3">
         <v>2200000</v>
@@ -22424,7 +22573,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -22432,108 +22581,12 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B5">
         <f>B1*(1+(B2/B3))-B4*(B2/B3)</f>
         <v>1.4098999999999999</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.25" customWidth="1"/>
-    <col min="3" max="3" width="46.75" customWidth="1"/>
-    <col min="4" max="4" width="16.375" customWidth="1"/>
-    <col min="5" max="5" width="30.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="30">
-        <v>44223</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>192</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>193</v>
-      </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
It was included new structure to store data on FLASH
</commit_message>
<xml_diff>
--- a/CDI_code/Hardware/Hardware_Description_v2.xlsx
+++ b/CDI_code/Hardware/Hardware_Description_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev_Fabio\CDIrepo\CDI_code\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\BACKUP\CDIrepo\CDI_code\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F18DBC-C191-45DB-B5D8-8D84C1A9D9AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EAC3DA-D4E5-4069-B756-800050CD97CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="2" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="276">
   <si>
     <t xml:space="preserve">Story </t>
   </si>
@@ -868,9 +868,6 @@
     <t>Temperature sensor</t>
   </si>
   <si>
-    <t>Create a code responsible to treat the temperature sensor (NTC resistor), create an array with 8 position to describe the temperature in function the voltage on resistor</t>
-  </si>
-  <si>
     <t>Update all documentation to create a efficient historic about the project, hardware details (include a possibility to include a E2PROM I2C memory on the board), redraw the GND regarding VRS sensor and stuff</t>
   </si>
   <si>
@@ -887,6 +884,30 @@
   </si>
   <si>
     <t xml:space="preserve">Finish the aluminum box (cut and conncet the internal wires) </t>
+  </si>
+  <si>
+    <t>Create a code responsible to treat the temperature sensor (NTC resistor), create an array with 12 position to describe the temperature in function the voltage on resistor</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Include more calibration parameters</t>
+  </si>
+  <si>
+    <t>Try to bring up new parameters to include in the calibration set like Sensor Characteristics, Engine Speed Limit and others</t>
+  </si>
+  <si>
+    <t>Improving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a trigger to record data on FLASH </t>
+  </si>
+  <si>
+    <t>I need to understand in details regarding which data I need to record on FLASH and when, because I can´t disturb the system during this process</t>
+  </si>
+  <si>
+    <t>tackle the obstacles</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1277,6 +1298,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8806,19 +8833,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.25" customWidth="1"/>
-    <col min="3" max="3" width="46.75" customWidth="1"/>
-    <col min="4" max="4" width="16.375" customWidth="1"/>
-    <col min="5" max="5" width="30.875" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.7265625" customWidth="1"/>
+    <col min="4" max="4" width="16.36328125" customWidth="1"/>
+    <col min="5" max="5" width="30.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -8841,7 +8868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="88.2" x14ac:dyDescent="0.2">
       <c r="A2" s="30">
         <v>44502</v>
       </c>
@@ -8851,11 +8878,13 @@
       <c r="C2" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="D2" s="31"/>
+      <c r="D2" s="65" t="s">
+        <v>272</v>
+      </c>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
     </row>
-    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="50.4" x14ac:dyDescent="0.2">
       <c r="A3" s="30">
         <v>44502</v>
       </c>
@@ -8863,61 +8892,88 @@
         <v>261</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>262</v>
-      </c>
-      <c r="D3" s="31"/>
+        <v>268</v>
+      </c>
+      <c r="D3" s="65" t="s">
+        <v>269</v>
+      </c>
       <c r="E3" s="31"/>
       <c r="F3" s="31"/>
     </row>
-    <row r="4" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="50.4" x14ac:dyDescent="0.2">
       <c r="A4" s="30">
         <v>44502</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>263</v>
-      </c>
-      <c r="D4" s="31"/>
+        <v>262</v>
+      </c>
+      <c r="D4" s="65"/>
       <c r="E4" s="31"/>
       <c r="F4" s="31"/>
     </row>
-    <row r="5" spans="1:6" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="75.599999999999994" x14ac:dyDescent="0.2">
       <c r="A5" s="30">
         <v>44502</v>
       </c>
       <c r="B5" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="C5" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="C5" s="32" t="s">
-        <v>266</v>
-      </c>
-      <c r="D5" s="31"/>
+      <c r="D5" s="65"/>
       <c r="E5" s="31"/>
       <c r="F5" s="31"/>
     </row>
-    <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="25.2" x14ac:dyDescent="0.2">
       <c r="A6" s="30">
         <v>44502</v>
       </c>
       <c r="B6" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="C6" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="C6" s="32" t="s">
-        <v>268</v>
-      </c>
-      <c r="D6" s="31"/>
+      <c r="D6" s="65"/>
       <c r="E6" s="31"/>
       <c r="F6" s="31"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+    <row r="7" spans="1:6" ht="37.799999999999997" x14ac:dyDescent="0.2">
+      <c r="A7" s="30">
+        <v>44504</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="D7" s="65"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+    </row>
+    <row r="8" spans="1:6" ht="37.799999999999997" x14ac:dyDescent="0.2">
+      <c r="A8" s="30">
+        <v>44504</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="D8" s="65"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C10" s="66" t="s">
+        <v>275</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8933,7 +8989,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -9009,26 +9065,26 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11646,7 +11702,7 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
@@ -12823,26 +12879,26 @@
       <selection sqref="A1:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15460,15 +15516,15 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -16495,16 +16551,16 @@
       <selection activeCell="D6" sqref="D6:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.90625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -20875,14 +20931,14 @@
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.625" customWidth="1"/>
+    <col min="1" max="1" width="3.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -21667,7 +21723,7 @@
       <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="49" t="s">
@@ -22039,7 +22095,7 @@
         <v>0.18666666666666668</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="44">
         <v>4.6199999999999998E-2</v>
       </c>
@@ -22181,10 +22237,10 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -22323,9 +22379,9 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -22428,7 +22484,7 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -22545,7 +22601,7 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -22602,16 +22658,16 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.875" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" customWidth="1"/>
+    <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.90625" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -23738,16 +23794,16 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.875" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" customWidth="1"/>
+    <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.90625" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Í cleaned the code, include new parameter in Calibration(Edge)
</commit_message>
<xml_diff>
--- a/CDI_code/Hardware/Hardware_Description_v2.xlsx
+++ b/CDI_code/Hardware/Hardware_Description_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\BACKUP\CDIrepo\CDI_code\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EAC3DA-D4E5-4069-B756-800050CD97CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB803FEB-010E-4342-BDBB-D4DC9D9F68C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="2" r:id="rId1"/>
@@ -1251,6 +1251,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1298,12 +1304,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8246,6 +8246,72 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>769620</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EDBEF17-737C-408D-A5A2-B08B41BEFC68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6286500" y="2339340"/>
+          <a:ext cx="5974080" cy="2194560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>358140</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -8308,7 +8374,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -8374,7 +8440,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8415,7 +8481,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8458,7 +8524,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8499,7 +8565,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8542,7 +8608,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8835,7 +8901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -8878,7 +8944,7 @@
       <c r="C2" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="49" t="s">
         <v>272</v>
       </c>
       <c r="E2" s="31"/>
@@ -8894,7 +8960,7 @@
       <c r="C3" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="49" t="s">
         <v>269</v>
       </c>
       <c r="E3" s="31"/>
@@ -8910,7 +8976,7 @@
       <c r="C4" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="49"/>
       <c r="E4" s="31"/>
       <c r="F4" s="31"/>
     </row>
@@ -8924,7 +8990,7 @@
       <c r="C5" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="D5" s="65"/>
+      <c r="D5" s="49"/>
       <c r="E5" s="31"/>
       <c r="F5" s="31"/>
     </row>
@@ -8938,7 +9004,7 @@
       <c r="C6" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="D6" s="65"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="31"/>
       <c r="F6" s="31"/>
     </row>
@@ -8952,7 +9018,7 @@
       <c r="C7" s="32" t="s">
         <v>271</v>
       </c>
-      <c r="D7" s="65"/>
+      <c r="D7" s="49"/>
       <c r="E7" s="31"/>
       <c r="F7" s="31"/>
     </row>
@@ -8966,12 +9032,12 @@
       <c r="C8" s="32" t="s">
         <v>274</v>
       </c>
-      <c r="D8" s="65"/>
+      <c r="D8" s="49"/>
       <c r="E8" s="31"/>
       <c r="F8" s="31"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="50" t="s">
         <v>275</v>
       </c>
     </row>
@@ -15536,51 +15602,51 @@
       <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="52" t="s">
         <v>163</v>
       </c>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="53" t="s">
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="55" t="s">
         <v>170</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="56" t="s">
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="58"/>
-      <c r="AA1" s="59" t="s">
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="61" t="s">
         <v>177</v>
       </c>
-      <c r="AB1" s="60"/>
-      <c r="AC1" s="60"/>
-      <c r="AD1" s="60"/>
-      <c r="AE1" s="60"/>
-      <c r="AF1" s="61"/>
-      <c r="AG1" s="53" t="s">
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="55" t="s">
         <v>174</v>
       </c>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="55"/>
-      <c r="AM1" s="62" t="s">
+      <c r="AH1" s="56"/>
+      <c r="AI1" s="56"/>
+      <c r="AJ1" s="56"/>
+      <c r="AK1" s="56"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="64" t="s">
         <v>172</v>
       </c>
-      <c r="AN1" s="63"/>
-      <c r="AO1" s="63"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="64"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="66"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -16572,51 +16638,51 @@
       <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="52" t="s">
         <v>163</v>
       </c>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="53" t="s">
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="55" t="s">
         <v>170</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="56" t="s">
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="58"/>
-      <c r="AA1" s="59" t="s">
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="61" t="s">
         <v>177</v>
       </c>
-      <c r="AB1" s="60"/>
-      <c r="AC1" s="60"/>
-      <c r="AD1" s="60"/>
-      <c r="AE1" s="60"/>
-      <c r="AF1" s="61"/>
-      <c r="AG1" s="53" t="s">
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="55" t="s">
         <v>174</v>
       </c>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="55"/>
-      <c r="AM1" s="62" t="s">
+      <c r="AH1" s="56"/>
+      <c r="AI1" s="56"/>
+      <c r="AJ1" s="56"/>
+      <c r="AK1" s="56"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="64" t="s">
         <v>172</v>
       </c>
-      <c r="AN1" s="63"/>
-      <c r="AO1" s="63"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="64"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="66"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -20927,8 +20993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -21712,6 +21778,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -21726,10 +21793,10 @@
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Í cleaned the code, included new parameter in Calibration(Edge) and fix the calibration software
</commit_message>
<xml_diff>
--- a/CDI_code/Hardware/Hardware_Description_v2.xlsx
+++ b/CDI_code/Hardware/Hardware_Description_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\BACKUP\CDIrepo\CDI_code\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EAC3DA-D4E5-4069-B756-800050CD97CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB803FEB-010E-4342-BDBB-D4DC9D9F68C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="2" r:id="rId1"/>
@@ -1251,6 +1251,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1298,12 +1304,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8246,6 +8246,72 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>769620</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EDBEF17-737C-408D-A5A2-B08B41BEFC68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6286500" y="2339340"/>
+          <a:ext cx="5974080" cy="2194560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>358140</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -8308,7 +8374,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -8374,7 +8440,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8415,7 +8481,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8458,7 +8524,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8499,7 +8565,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8542,7 +8608,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8835,7 +8901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -8878,7 +8944,7 @@
       <c r="C2" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="49" t="s">
         <v>272</v>
       </c>
       <c r="E2" s="31"/>
@@ -8894,7 +8960,7 @@
       <c r="C3" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="49" t="s">
         <v>269</v>
       </c>
       <c r="E3" s="31"/>
@@ -8910,7 +8976,7 @@
       <c r="C4" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="49"/>
       <c r="E4" s="31"/>
       <c r="F4" s="31"/>
     </row>
@@ -8924,7 +8990,7 @@
       <c r="C5" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="D5" s="65"/>
+      <c r="D5" s="49"/>
       <c r="E5" s="31"/>
       <c r="F5" s="31"/>
     </row>
@@ -8938,7 +9004,7 @@
       <c r="C6" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="D6" s="65"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="31"/>
       <c r="F6" s="31"/>
     </row>
@@ -8952,7 +9018,7 @@
       <c r="C7" s="32" t="s">
         <v>271</v>
       </c>
-      <c r="D7" s="65"/>
+      <c r="D7" s="49"/>
       <c r="E7" s="31"/>
       <c r="F7" s="31"/>
     </row>
@@ -8966,12 +9032,12 @@
       <c r="C8" s="32" t="s">
         <v>274</v>
       </c>
-      <c r="D8" s="65"/>
+      <c r="D8" s="49"/>
       <c r="E8" s="31"/>
       <c r="F8" s="31"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="50" t="s">
         <v>275</v>
       </c>
     </row>
@@ -15536,51 +15602,51 @@
       <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="52" t="s">
         <v>163</v>
       </c>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="53" t="s">
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="55" t="s">
         <v>170</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="56" t="s">
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="58"/>
-      <c r="AA1" s="59" t="s">
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="61" t="s">
         <v>177</v>
       </c>
-      <c r="AB1" s="60"/>
-      <c r="AC1" s="60"/>
-      <c r="AD1" s="60"/>
-      <c r="AE1" s="60"/>
-      <c r="AF1" s="61"/>
-      <c r="AG1" s="53" t="s">
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="55" t="s">
         <v>174</v>
       </c>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="55"/>
-      <c r="AM1" s="62" t="s">
+      <c r="AH1" s="56"/>
+      <c r="AI1" s="56"/>
+      <c r="AJ1" s="56"/>
+      <c r="AK1" s="56"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="64" t="s">
         <v>172</v>
       </c>
-      <c r="AN1" s="63"/>
-      <c r="AO1" s="63"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="64"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="66"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -16572,51 +16638,51 @@
       <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="52" t="s">
         <v>163</v>
       </c>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="53" t="s">
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="55" t="s">
         <v>170</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="56" t="s">
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="58"/>
-      <c r="AA1" s="59" t="s">
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="61" t="s">
         <v>177</v>
       </c>
-      <c r="AB1" s="60"/>
-      <c r="AC1" s="60"/>
-      <c r="AD1" s="60"/>
-      <c r="AE1" s="60"/>
-      <c r="AF1" s="61"/>
-      <c r="AG1" s="53" t="s">
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="55" t="s">
         <v>174</v>
       </c>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="55"/>
-      <c r="AM1" s="62" t="s">
+      <c r="AH1" s="56"/>
+      <c r="AI1" s="56"/>
+      <c r="AJ1" s="56"/>
+      <c r="AK1" s="56"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="64" t="s">
         <v>172</v>
       </c>
-      <c r="AN1" s="63"/>
-      <c r="AO1" s="63"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="64"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="66"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
@@ -20927,8 +20993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -21712,6 +21778,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -21726,10 +21793,10 @@
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="51" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">

</xml_diff>

<commit_message>
Some basic code organization, and update backlog
</commit_message>
<xml_diff>
--- a/CDI_code/Hardware/Hardware_Description_v2.xlsx
+++ b/CDI_code/Hardware/Hardware_Description_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\BACKUP\CDIrepo\CDI_code\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB803FEB-010E-4342-BDBB-D4DC9D9F68C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8330F7-6710-4459-95DF-224CBC212FAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="2" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="284">
   <si>
     <t xml:space="preserve">Story </t>
   </si>
@@ -883,9 +883,6 @@
     <t>Final product (Box and assembly)</t>
   </si>
   <si>
-    <t xml:space="preserve">Finish the aluminum box (cut and conncet the internal wires) </t>
-  </si>
-  <si>
     <t>Create a code responsible to treat the temperature sensor (NTC resistor), create an array with 12 position to describe the temperature in function the voltage on resistor</t>
   </si>
   <si>
@@ -908,6 +905,33 @@
   </si>
   <si>
     <t>tackle the obstacles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish the aluminum box (cut and connect the internal wires) </t>
+  </si>
+  <si>
+    <t>It was done with some limitations (I need to create trigger to record this data on FLASH)</t>
+  </si>
+  <si>
+    <t>Create a hardware validation</t>
+  </si>
+  <si>
+    <t>I need to elaborate some hardware validation process to validate de circuit, I need to prepare the stick to glue on disc (graduate degrees division)</t>
+  </si>
+  <si>
+    <t>Buy the components to assembly some CDI and try to distribute</t>
+  </si>
+  <si>
+    <t>Is important thing respect this, because I need to validate this circuit in some vehicle to get confidence in the circuit and sw…</t>
+  </si>
+  <si>
+    <t>*Finish the CDI case, activate the WDT inside the sw and prepare some basic sinalization to prepare the CDI to be operated for someone…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read basic information </t>
+  </si>
+  <si>
+    <t>Prepare basic tool set to send and read calibration, read and clear system data</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1304,6 +1328,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8899,10 +8926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -8945,7 +8972,7 @@
         <v>260</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
@@ -8958,10 +8985,10 @@
         <v>261</v>
       </c>
       <c r="C3" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="D3" s="49" t="s">
         <v>268</v>
-      </c>
-      <c r="D3" s="49" t="s">
-        <v>269</v>
       </c>
       <c r="E3" s="31"/>
       <c r="F3" s="31"/>
@@ -8990,8 +9017,12 @@
       <c r="C5" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="31"/>
+      <c r="D5" s="49" t="s">
+        <v>268</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>276</v>
+      </c>
       <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" ht="25.2" x14ac:dyDescent="0.2">
@@ -9002,7 +9033,7 @@
         <v>266</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="D6" s="49"/>
       <c r="E6" s="31"/>
@@ -9013,10 +9044,10 @@
         <v>44504</v>
       </c>
       <c r="B7" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="C7" s="32" t="s">
         <v>270</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>271</v>
       </c>
       <c r="D7" s="49"/>
       <c r="E7" s="31"/>
@@ -9027,18 +9058,68 @@
         <v>44504</v>
       </c>
       <c r="B8" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="C8" s="32" t="s">
         <v>273</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>274</v>
       </c>
       <c r="D8" s="49"/>
       <c r="E8" s="31"/>
       <c r="F8" s="31"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C10" s="50" t="s">
-        <v>275</v>
+    <row r="9" spans="1:6" ht="37.799999999999997" x14ac:dyDescent="0.2">
+      <c r="A9" s="30">
+        <v>44515</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="D9" s="49"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+    </row>
+    <row r="10" spans="1:6" ht="37.799999999999997" x14ac:dyDescent="0.2">
+      <c r="A10" s="30">
+        <v>44515</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="D10" s="49"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+    </row>
+    <row r="11" spans="1:6" ht="63" x14ac:dyDescent="0.2">
+      <c r="A11" s="30">
+        <v>44515</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="C11" s="32"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+    </row>
+    <row r="12" spans="1:6" ht="37.799999999999997" x14ac:dyDescent="0.2">
+      <c r="B12" s="67" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="67" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C20" s="50" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -20993,7 +21074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>

</xml_diff>